<commit_message>
Calling a Java Class from JSP
</commit_message>
<xml_diff>
--- a/me_docs/2.JSP-Fundamentals.xlsx
+++ b/me_docs/2.JSP-Fundamentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EEF50F-44E8-4DF2-B3A3-589CEC77463E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A287138C-6826-460F-B797-0162527E9F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fix eror" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Expressions" sheetId="3" r:id="rId3"/>
     <sheet name="Scriptlets" sheetId="4" r:id="rId4"/>
     <sheet name="Declarations" sheetId="6" r:id="rId5"/>
+    <sheet name="Calling a Java Class from JSP" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Create Dynamic Web Project</t>
   </si>
@@ -94,6 +95,18 @@
   </si>
   <si>
     <t>Create declaration-test.jsp</t>
+  </si>
+  <si>
+    <t>Create Package com.luv2code.jsp</t>
+  </si>
+  <si>
+    <t>Create class FunUtils</t>
+  </si>
+  <si>
+    <t>Create fun-test.jsp</t>
+  </si>
+  <si>
+    <t>Acess url to test: http://localhost:8080/jspdemo/fun-test.jsp</t>
   </si>
 </sst>
 </file>
@@ -1183,6 +1196,407 @@
         <a:xfrm>
           <a:off x="609600" y="15621000"/>
           <a:ext cx="4923809" cy="1276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>170590</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>27952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5486A61-564B-420F-8FE7-424B035563C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1143000"/>
+          <a:ext cx="6876190" cy="4980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>56643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{287DD2D0-DDA5-44D8-BEAD-C3B32746A4E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6286500"/>
+          <a:ext cx="4866667" cy="4057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>418209</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>113881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0C2A1C-1A29-40EB-8F62-65BD08CF60C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="10096500"/>
+          <a:ext cx="7123809" cy="3352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>151771</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>104024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDAE6E73-79B3-4E23-980D-0980AB4E6B8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="13716000"/>
+          <a:ext cx="5028571" cy="6009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D87CF67-FB91-45D1-87C8-94923034D3A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20193000"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>151690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F9E2938-43B2-43A7-B4BE-354390012AC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="25146000"/>
+          <a:ext cx="4876190" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>599238</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>9119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{986B4787-6717-43CB-84FB-D98C3027EC1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20002500"/>
+          <a:ext cx="6695238" cy="3247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>284800</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>28024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC22F55D-79CE-4A90-9AB2-CACA8803908E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="34671000"/>
+          <a:ext cx="7600000" cy="4409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>275733</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>104571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61CF5268-4070-483C-84E3-30FC9A4C3CFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="39624000"/>
+          <a:ext cx="3933333" cy="1628571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1603,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F234B01-DED5-4AFD-93B0-27D013411CD8}">
   <dimension ref="A3:A82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,4 +2042,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636875A8-FC73-4A12-A9D2-41431C04E253}">
+  <dimension ref="A2:A208"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Including Files in JSP
</commit_message>
<xml_diff>
--- a/me_docs/2.JSP-Fundamentals.xlsx
+++ b/me_docs/2.JSP-Fundamentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3892073E-6FEF-4C39-A187-3C25959C17E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259BB3C8-E7D3-4B3D-BFAB-FEF6F07A6BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fix eror" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Declarations" sheetId="6" r:id="rId5"/>
     <sheet name="Calling a Java Class from JSP" sheetId="7" r:id="rId6"/>
     <sheet name="JSP Built-In Objects" sheetId="8" r:id="rId7"/>
+    <sheet name="Including Files in JSP" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Create Dynamic Web Project</t>
   </si>
@@ -120,6 +121,21 @@
   </si>
   <si>
     <t>Acess url to test: http://localhost:8080/jspdemo/builtin-test.jsp</t>
+  </si>
+  <si>
+    <t>Create my-header.html</t>
+  </si>
+  <si>
+    <t>my-header.html</t>
+  </si>
+  <si>
+    <t>Create my-footer.jsp</t>
+  </si>
+  <si>
+    <t>Create homepage.jsp</t>
+  </si>
+  <si>
+    <t>Acess url to test: http://localhost:8080/jspdemo/homepage.jsp</t>
   </si>
 </sst>
 </file>
@@ -1800,6 +1816,451 @@
         <a:xfrm>
           <a:off x="609600" y="16764000"/>
           <a:ext cx="9914286" cy="1742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D0AAC6-7D3D-48C9-87A7-48AE1AC3D85B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>580419</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>161214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C645BC-019C-4CC1-BC30-0B7AD44003E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="4847619" cy="5685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>30964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{756D2F83-59FC-4094-9F48-5BC8A3A496E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11430000"/>
+          <a:ext cx="6143625" cy="4602964"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F811A71-ADCE-452F-8DE2-CC7FE1A8789F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16573500"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E896DE5-22AD-4C10-9AFF-ABECBC379F67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21526500"/>
+          <a:ext cx="4866667" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>551467</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>113667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C41DC46-17C2-449C-8F2F-16B2C4C5E2E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="27432000"/>
+          <a:ext cx="7866667" cy="5066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65828</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE24549-E8CE-4DD9-B01F-0C1543DBEBCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32956500"/>
+          <a:ext cx="6771428" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>151690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4DBE9BB-F837-4B50-AC6E-516FA27F0E57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="37909500"/>
+          <a:ext cx="4885714" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>379962</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>27929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98875871-10C2-4413-BA66-064E667742C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="43815000"/>
+          <a:ext cx="8304762" cy="5171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>322819</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>47286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98CEBA7-5BBA-49AC-AE76-964DF0D4DFA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="49530000"/>
+          <a:ext cx="8247619" cy="2714286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2287,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BB6D83-DA82-4A49-860A-5F0DD4BD514D}">
   <dimension ref="A2:A88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,4 +2779,46 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87266AB-FECF-426D-97A2-B2C6E2F3156E}">
+  <dimension ref="A2:A260"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="R268" sqref="R268"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>